<commit_message>
new changes done on 6 April
</commit_message>
<xml_diff>
--- a/UploadExcel/ProviderDataUploadTemplate.xlsx
+++ b/UploadExcel/ProviderDataUploadTemplate.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="165" uniqueCount="88">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="183" uniqueCount="93">
   <si>
     <t>Name</t>
   </si>
@@ -264,9 +264,6 @@
     <t>Irfan</t>
   </si>
   <si>
-    <t>test</t>
-  </si>
-  <si>
     <t>ServiceProviderCode</t>
   </si>
   <si>
@@ -289,6 +286,24 @@
   </si>
   <si>
     <t>New</t>
+  </si>
+  <si>
+    <t>AB001</t>
+  </si>
+  <si>
+    <t>test change</t>
+  </si>
+  <si>
+    <t>NE001</t>
+  </si>
+  <si>
+    <t>Check</t>
+  </si>
+  <si>
+    <t>June</t>
+  </si>
+  <si>
+    <t>New123</t>
   </si>
 </sst>
 </file>
@@ -651,10 +666,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I16"/>
+  <dimension ref="A1:I18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H17" sqref="H17"/>
+      <selection activeCell="F17" sqref="F17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -673,7 +688,7 @@
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>0</v>
@@ -708,7 +723,7 @@
         <v>12</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="D2" s="2" t="s">
         <v>34</v>
@@ -737,7 +752,7 @@
         <v>17</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="D3" s="2" t="s">
         <v>34</v>
@@ -749,7 +764,7 @@
         <v>11</v>
       </c>
       <c r="G3" s="7" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="H3" s="2" t="s">
         <v>15</v>
@@ -778,7 +793,7 @@
         <v>23</v>
       </c>
       <c r="G4" s="7" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="H4" s="2" t="s">
         <v>10</v>
@@ -795,7 +810,7 @@
         <v>25</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="D5" s="2" t="s">
         <v>32</v>
@@ -836,7 +851,7 @@
         <v>11</v>
       </c>
       <c r="G6" s="7" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="H6" s="2" t="s">
         <v>35</v>
@@ -911,7 +926,7 @@
         <v>45</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="D9" s="2" t="s">
         <v>31</v>
@@ -923,7 +938,7 @@
         <v>39</v>
       </c>
       <c r="G9" s="7" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="H9" s="2" t="s">
         <v>10</v>
@@ -969,7 +984,7 @@
         <v>51</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="D11" s="2" t="s">
         <v>31</v>
@@ -981,7 +996,7 @@
         <v>11</v>
       </c>
       <c r="G11" s="7" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="H11" s="2" t="s">
         <v>15</v>
@@ -998,7 +1013,7 @@
         <v>54</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="D12" s="8" t="s">
         <v>56</v>
@@ -1010,7 +1025,7 @@
         <v>57</v>
       </c>
       <c r="G12" s="7" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="H12" s="2" t="s">
         <v>15</v>
@@ -1094,7 +1109,7 @@
         <v>8</v>
       </c>
       <c r="F15" s="2" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="G15" s="5" t="s">
         <v>43</v>
@@ -1114,7 +1129,7 @@
         <v>76</v>
       </c>
       <c r="C16" s="2" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="D16" s="2" t="s">
         <v>77</v>
@@ -1123,16 +1138,74 @@
         <v>78</v>
       </c>
       <c r="F16" s="2" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="G16" s="7" t="s">
         <v>43</v>
       </c>
       <c r="H16" s="2" t="s">
+        <v>86</v>
+      </c>
+      <c r="I16" s="2" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A17" s="3" t="s">
         <v>87</v>
       </c>
-      <c r="I16" s="2" t="s">
-        <v>79</v>
+      <c r="B17" s="2" t="s">
+        <v>92</v>
+      </c>
+      <c r="C17" s="2" t="s">
+        <v>84</v>
+      </c>
+      <c r="D17" s="2" t="s">
+        <v>77</v>
+      </c>
+      <c r="E17" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="F17" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="G17" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="H17" s="2" t="s">
+        <v>86</v>
+      </c>
+      <c r="I17" s="2" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A18" s="3" t="s">
+        <v>89</v>
+      </c>
+      <c r="B18" s="2" t="s">
+        <v>90</v>
+      </c>
+      <c r="C18" s="2" t="s">
+        <v>86</v>
+      </c>
+      <c r="D18" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="E18" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="F18" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="G18" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="H18" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="I18" s="2" t="s">
+        <v>90</v>
       </c>
     </row>
   </sheetData>
@@ -1157,7 +1230,7 @@
   <dimension ref="A1:E10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
+      <selection activeCell="A5" sqref="A5:XFD5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1171,7 +1244,7 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>0</v>
@@ -1231,10 +1304,10 @@
         <v>2</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="E4" s="3" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
@@ -1248,7 +1321,7 @@
         <v>1</v>
       </c>
       <c r="D5" s="3" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="E5" s="3" t="s">
         <v>78</v>

</xml_diff>

<commit_message>
new changes on 7 April
</commit_message>
<xml_diff>
--- a/UploadExcel/ProviderDataUploadTemplate.xlsx
+++ b/UploadExcel/ProviderDataUploadTemplate.xlsx
@@ -12,7 +12,7 @@
     <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7620"/>
   </bookViews>
   <sheets>
-    <sheet name="ServiceProviderList" sheetId="1" r:id="rId1"/>
+    <sheet name="ProviderList" sheetId="1" r:id="rId1"/>
     <sheet name="IssueList" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="162913"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="183" uniqueCount="93">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="192" uniqueCount="96">
   <si>
     <t>Name</t>
   </si>
@@ -264,9 +264,6 @@
     <t>Irfan</t>
   </si>
   <si>
-    <t>ServiceProviderCode</t>
-  </si>
-  <si>
     <t>Test Owner</t>
   </si>
   <si>
@@ -304,6 +301,18 @@
   </si>
   <si>
     <t>New123</t>
+  </si>
+  <si>
+    <t>NN012</t>
+  </si>
+  <si>
+    <t>test provider</t>
+  </si>
+  <si>
+    <t>chech provider date</t>
+  </si>
+  <si>
+    <t>VendorCode</t>
   </si>
 </sst>
 </file>
@@ -666,10 +675,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I18"/>
+  <dimension ref="A1:I19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F17" sqref="F17"/>
+      <selection activeCell="D21" sqref="D21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -688,7 +697,7 @@
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>79</v>
+        <v>95</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>0</v>
@@ -723,7 +732,7 @@
         <v>12</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="D2" s="2" t="s">
         <v>34</v>
@@ -752,7 +761,7 @@
         <v>17</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="D3" s="2" t="s">
         <v>34</v>
@@ -764,7 +773,7 @@
         <v>11</v>
       </c>
       <c r="G3" s="7" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="H3" s="2" t="s">
         <v>15</v>
@@ -793,7 +802,7 @@
         <v>23</v>
       </c>
       <c r="G4" s="7" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="H4" s="2" t="s">
         <v>10</v>
@@ -810,7 +819,7 @@
         <v>25</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="D5" s="2" t="s">
         <v>32</v>
@@ -851,7 +860,7 @@
         <v>11</v>
       </c>
       <c r="G6" s="7" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="H6" s="2" t="s">
         <v>35</v>
@@ -926,7 +935,7 @@
         <v>45</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="D9" s="2" t="s">
         <v>31</v>
@@ -938,7 +947,7 @@
         <v>39</v>
       </c>
       <c r="G9" s="7" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="H9" s="2" t="s">
         <v>10</v>
@@ -984,7 +993,7 @@
         <v>51</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="D11" s="2" t="s">
         <v>31</v>
@@ -996,7 +1005,7 @@
         <v>11</v>
       </c>
       <c r="G11" s="7" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="H11" s="2" t="s">
         <v>15</v>
@@ -1013,7 +1022,7 @@
         <v>54</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="D12" s="8" t="s">
         <v>56</v>
@@ -1025,7 +1034,7 @@
         <v>57</v>
       </c>
       <c r="G12" s="7" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="H12" s="2" t="s">
         <v>15</v>
@@ -1109,7 +1118,7 @@
         <v>8</v>
       </c>
       <c r="F15" s="2" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="G15" s="5" t="s">
         <v>43</v>
@@ -1129,7 +1138,7 @@
         <v>76</v>
       </c>
       <c r="C16" s="2" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="D16" s="2" t="s">
         <v>77</v>
@@ -1138,27 +1147,27 @@
         <v>78</v>
       </c>
       <c r="F16" s="2" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="G16" s="7" t="s">
         <v>43</v>
       </c>
       <c r="H16" s="2" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="I16" s="2" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A17" s="3" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="C17" s="2" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="D17" s="2" t="s">
         <v>77</v>
@@ -1173,24 +1182,24 @@
         <v>43</v>
       </c>
       <c r="H17" s="2" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="I17" s="2" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A18" s="3" t="s">
+        <v>88</v>
+      </c>
+      <c r="B18" s="2" t="s">
         <v>89</v>
       </c>
-      <c r="B18" s="2" t="s">
+      <c r="C18" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="D18" s="2" t="s">
         <v>90</v>
-      </c>
-      <c r="C18" s="2" t="s">
-        <v>86</v>
-      </c>
-      <c r="D18" s="2" t="s">
-        <v>91</v>
       </c>
       <c r="E18" s="2" t="s">
         <v>8</v>
@@ -1205,7 +1214,36 @@
         <v>15</v>
       </c>
       <c r="I18" s="2" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A19" s="3" t="s">
+        <v>92</v>
+      </c>
+      <c r="B19" s="2" t="s">
+        <v>93</v>
+      </c>
+      <c r="C19" s="2" t="s">
+        <v>83</v>
+      </c>
+      <c r="D19" s="2" t="s">
         <v>90</v>
+      </c>
+      <c r="E19" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="F19" s="2" t="s">
+        <v>84</v>
+      </c>
+      <c r="G19" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="H19" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="I19" s="2" t="s">
+        <v>94</v>
       </c>
     </row>
   </sheetData>
@@ -1230,7 +1268,7 @@
   <dimension ref="A1:E10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A5" sqref="A5:XFD5"/>
+      <selection activeCell="B18" sqref="B18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1244,7 +1282,7 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>79</v>
+        <v>95</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>0</v>
@@ -1304,10 +1342,10 @@
         <v>2</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="E4" s="3" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
@@ -1321,7 +1359,7 @@
         <v>1</v>
       </c>
       <c r="D5" s="3" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="E5" s="3" t="s">
         <v>78</v>

</xml_diff>